<commit_message>
testng and data driven test with dataprovider step 1
</commit_message>
<xml_diff>
--- a/ExcelFile/logindata.xlsx
+++ b/ExcelFile/logindata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22208"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEB9917B-3AE9-42FC-8949-46432AFDE808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD3DDBBB-EFD5-4FCE-ABE6-7E725AA13DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>DataNo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>CaseNo</t>
   </si>
   <si>
     <t>Username</t>
@@ -34,10 +34,46 @@
     <t>Password</t>
   </si>
   <si>
-    <t>xyaerdjs@gmail.com</t>
-  </si>
-  <si>
-    <t>aekfjd@gmail.com</t>
+    <t>Case1</t>
+  </si>
+  <si>
+    <t>oglcnarbc@gmail.com</t>
+  </si>
+  <si>
+    <t>Case2</t>
+  </si>
+  <si>
+    <t>1a8BA</t>
+  </si>
+  <si>
+    <t>Case3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Case4</t>
+  </si>
+  <si>
+    <t>oglcnarbc</t>
+  </si>
+  <si>
+    <t>Case5</t>
+  </si>
+  <si>
+    <t>oAb_13@gmail.com</t>
+  </si>
+  <si>
+    <t>3a54c</t>
+  </si>
+  <si>
+    <t>Case6</t>
+  </si>
+  <si>
+    <t>555b@g.co</t>
+  </si>
+  <si>
+    <t>Case7</t>
   </si>
 </sst>
 </file>
@@ -400,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,31 +459,89 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1324</v>
+        <v>123456</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>121324</v>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F2FC2F3B-6ECD-4C90-8213-E0273134CA57}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{0A74A455-B216-4A60-98C2-668C58B52BD2}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A8E53B7A-874E-413F-B90D-6356BC8F3186}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{D366E086-4603-48C1-83CB-0ECF628145E7}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{3C276104-72AD-4E3D-B2E3-F05DDB09B50E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit excel data. added new user info
</commit_message>
<xml_diff>
--- a/ExcelFile/logindata.xlsx
+++ b/ExcelFile/logindata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22208"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD3DDBBB-EFD5-4FCE-ABE6-7E725AA13DBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45CBCF6A-6AB9-4043-AC76-B15E6C30048F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>CaseNo</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Case2</t>
+  </si>
+  <si>
+    <t>ogulcan.a81@hotmail.com</t>
   </si>
   <si>
     <t>1a8BA</t>
@@ -439,7 +442,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,29 +477,29 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>123456</v>
@@ -504,21 +507,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>123456</v>
@@ -526,10 +529,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>123456</v>

</xml_diff>

<commit_message>
some refactor and review :)
</commit_message>
<xml_diff>
--- a/ExcelFile/logindata.xlsx
+++ b/ExcelFile/logindata.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22208"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45CBCF6A-6AB9-4043-AC76-B15E6C30048F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A21B8096-2D49-4DEF-8F96-5E892B372D7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logindata" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Test Case" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -23,60 +24,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+  <si>
+    <t>DataNo</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>oglcnarbc@gmail.com</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>ogulcan.a81@hotmail.com</t>
+  </si>
+  <si>
+    <t>1a8BA</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>oglcnarbc</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>oAb_13@gmail.com</t>
+  </si>
+  <si>
+    <t>3a54c</t>
+  </si>
+  <si>
+    <t>Data6</t>
+  </si>
+  <si>
+    <t>555b@g.co</t>
+  </si>
+  <si>
+    <t>Data7</t>
+  </si>
   <si>
     <t>CaseNo</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
   </si>
   <si>
     <t>Case1</t>
   </si>
   <si>
-    <t>oglcnarbc@gmail.com</t>
+    <t>Doğru Kullanıcı adı ve Şifre girilir.</t>
+  </si>
+  <si>
+    <t>Login olunduğu görülür</t>
   </si>
   <si>
     <t>Case2</t>
   </si>
   <si>
-    <t>ogulcan.a81@hotmail.com</t>
-  </si>
-  <si>
-    <t>1a8BA</t>
+    <t>Yanlılş Kullanıcı adı ve Şifre girilir.</t>
+  </si>
+  <si>
+    <t>"Hatalı E-Posta / Şifre. Tekrar Deneyin." mesajı geldiği görülür</t>
   </si>
   <si>
     <t>Case3</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Doğru Kullanıcı ad ve Boş şifre girilir.</t>
+  </si>
+  <si>
+    <t>"Lütfen şifre giriniz." mesajının geldiği görülür</t>
   </si>
   <si>
     <t>Case4</t>
   </si>
   <si>
-    <t>oglcnarbc</t>
-  </si>
-  <si>
-    <t>Case5</t>
-  </si>
-  <si>
-    <t>oAb_13@gmail.com</t>
-  </si>
-  <si>
-    <t>3a54c</t>
-  </si>
-  <si>
-    <t>Case6</t>
-  </si>
-  <si>
-    <t>555b@g.co</t>
-  </si>
-  <si>
-    <t>Case7</t>
+    <t>Boş Kullanıcı adı ve Doğru şifre girilir.</t>
+  </si>
+  <si>
+    <t>"Lütfen email adresinizi giriniz." mesajının geldiği görülür</t>
   </si>
 </sst>
 </file>
@@ -442,7 +488,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -548,4 +594,78 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDAD714-591D-4F96-B9C2-5128BC533416}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>